<commit_message>
add route on server_target
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PFSense-OpenVPN-OpenStack-TUN" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="44">
   <si>
     <t>eth0</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>20.20.20.3</t>
+  </si>
+  <si>
+    <t>192.168.2.1</t>
   </si>
 </sst>
 </file>
@@ -750,7 +753,7 @@
   </sheetPr>
   <dimension ref="B2:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -1246,8 +1249,8 @@
   </sheetPr>
   <dimension ref="B2:N9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1425,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>11</v>
@@ -1513,14 +1516,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="B4:B6"/>
@@ -1531,6 +1526,14 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="N4:N6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>